<commit_message>
Added: Allows user to select file using a File Browser. Exceptions updated
</commit_message>
<xml_diff>
--- a/Excel Template/stow rate template.xlsx
+++ b/Excel Template/stow rate template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zache\Documents\GitHub\STRAP\Excel Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72CDB30-17BB-465E-9858-95ABC7242985}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{93A33CB1-903A-40CB-A6EB-2FA4FC3CC3CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -435,7 +435,7 @@
   <dimension ref="Q2:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G60" sqref="G60"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +453,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:C75">
+  <conditionalFormatting sqref="A1:C100">
     <cfRule type="expression" dxfId="4" priority="10">
       <formula>AND($C1&gt;5.9, $C1&lt;$R$2)</formula>
     </cfRule>
@@ -467,7 +467,7 @@
       <formula>AND($C1&gt;0, $C1&lt;2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:C75">
+  <conditionalFormatting sqref="A1:C100">
     <cfRule type="expression" dxfId="0" priority="14">
       <formula>$C1=$R$2</formula>
     </cfRule>

</xml_diff>